<commit_message>
criacao tabela regiao no tabelao
</commit_message>
<xml_diff>
--- a/Bases_IBGE/Tabelao_populacao2009-2018.xlsx
+++ b/Bases_IBGE/Tabelao_populacao2009-2018.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felipeclau\Documents\OPE\OPE_Imapcta\Bases_IBGE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB1A110-0C6D-42E1-BAAA-24F0CDA4291C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB54462F-AEF1-4F1C-A223-9D27C73C4614}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{D26A9040-84A3-4D87-9901-341F8A2FE85F}"/>
   </bookViews>
   <sheets>
     <sheet name="Junção tabelas" sheetId="1" r:id="rId1"/>
     <sheet name="F_Populacao" sheetId="3" r:id="rId2"/>
-    <sheet name="D_Calendario" sheetId="4" r:id="rId3"/>
-    <sheet name="D_UF" sheetId="2" r:id="rId4"/>
+    <sheet name="D_Regiao" sheetId="5" r:id="rId3"/>
+    <sheet name="D_Calendario" sheetId="4" r:id="rId4"/>
+    <sheet name="D_UF" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="41">
   <si>
     <t>Ano</t>
   </si>
@@ -157,6 +158,27 @@
   <si>
     <t>sk_Ano</t>
   </si>
+  <si>
+    <t>sk_Regiao</t>
+  </si>
+  <si>
+    <t>Regiao</t>
+  </si>
+  <si>
+    <t>Sul</t>
+  </si>
+  <si>
+    <t>Norte</t>
+  </si>
+  <si>
+    <t>Nordeste</t>
+  </si>
+  <si>
+    <t>Sudeste</t>
+  </si>
+  <si>
+    <t>Centro Oeste</t>
+  </si>
 </sst>
 </file>
 
@@ -164,9 +186,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,12 +202,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -212,7 +228,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,6 +451,14 @@
             <a:rPr lang="pt-BR" sz="1100" baseline="0"/>
             <a:t>6 - Criação tabela dimensão D_Calendário.</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" baseline="0"/>
+            <a:t>7 - Criação tabela dimensão D_Regiao</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
           <a:endParaRPr lang="pt-BR" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -451,6 +475,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{24BEF121-305D-44EF-9442-3936FA67A785}" name="D_Regiao" displayName="D_Regiao" ref="A2:B7" totalsRowShown="0">
+  <autoFilter ref="A2:B7" xr:uid="{7F3F46A2-D43C-477D-8066-39311FFEA005}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{B9DD0D33-AAD5-4932-B290-E0AD6D51B807}" name="sk_Regiao"/>
+    <tableColumn id="2" xr3:uid="{395A8DB4-32ED-4F5A-9D4D-7985E66FD9F4}" name="Regiao"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{380C67CA-C10C-4257-AEE9-489CE47546E4}" name="D_Calendario" displayName="D_Calendario" ref="A2:B12" totalsRowShown="0">
   <autoFilter ref="A2:B12" xr:uid="{6E0BECA7-EA2F-43B2-ACAC-D921D2AFC234}"/>
   <tableColumns count="2">
@@ -461,7 +496,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3ACF86D9-026A-4FAE-B648-3E082DC6CA67}" name="D_UF" displayName="D_UF" ref="A1:C28" totalsRowShown="0">
   <autoFilter ref="A1:C28" xr:uid="{60C492E7-7191-45BC-8A62-54AEAE5E0326}"/>
   <tableColumns count="3">
@@ -3782,7 +3817,7 @@
   <dimension ref="A2:E272"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8676,6 +8711,79 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43D99F3F-35D9-44A5-9C2D-6F41A2D0EA68}">
+  <dimension ref="A2:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.109375" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:B7">
+    <sortCondition ref="B3"/>
+  </sortState>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A2BAC22-5138-41EE-A266-1214CA1F2213}">
   <dimension ref="A2:B12"/>
   <sheetViews>
@@ -8781,7 +8889,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1F52DB7-7AD9-49AF-A732-C31369E98472}">
   <dimension ref="A1:C28"/>
   <sheetViews>

</xml_diff>